<commit_message>
axial MM podel osy z
mam problemy se skalou namerenych dat, u dat z brezna vychazi faktor 4, u dat z kvetna faktor 2.5 -- zkusim poradne zmerit
</commit_message>
<xml_diff>
--- a/EMM_minim/algoritmus minimalizace/EMM_min_pomocne_data.xlsx
+++ b/EMM_minim/algoritmus minimalizace/EMM_min_pomocne_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive_vut\ÚPT\diplomka\Julia_vypocty_diplomka\EMM_minim\algoritmus minimalizace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\škola-onedrive\OneDrive - Vysoké učení technické v Brně\ÚPT\diplomka\Julia_vypocty_diplomka\EMM_minim\algoritmus minimalizace\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_DF9832555ACC1ABA08EF7B8C364DAB2A8405147D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{828E5C82-30D8-4B97-A1D2-4461FEF52E87}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="15360" windowHeight="7545" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dark_res" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,17 @@
     <sheet name="citlivost" sheetId="5" r:id="rId5"/>
     <sheet name="nejistota histogramu" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -374,9 +385,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -429,7 +440,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +475,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -805,7 +815,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2250,7 +2259,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graf 1"/>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2280,7 +2295,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graf 3"/>
+        <xdr:cNvPr id="4" name="Graf 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2301,7 +2322,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2339,7 +2360,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2374,6 +2395,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2409,9 +2447,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2584,7 +2639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2705,7 +2760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:W54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4403,11 +4458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:N28"/>
+    <sheetView tabSelected="1" topLeftCell="Q31" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4602,6 +4657,9 @@
       <c r="U10">
         <v>1</v>
       </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
       <c r="W10">
         <v>0.316</v>
       </c>
@@ -4660,6 +4718,9 @@
       <c r="U11">
         <v>1</v>
       </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
       <c r="W11">
         <v>0.21</v>
       </c>
@@ -4702,14 +4763,14 @@
         <v>50</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O12:O28" si="0">(K13-L13)/(K13+L13)</f>
+        <f t="shared" ref="O13:O28" si="0">(K13-L13)/(K13+L13)</f>
         <v>0.16200000000000001</v>
       </c>
       <c r="P13">
         <v>256</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q12:Q28" si="1" xml:space="preserve"> $C$6/(I13-J13)</f>
+        <f t="shared" ref="Q13:Q28" si="1" xml:space="preserve"> $C$6/(I13-J13)</f>
         <v>102.73972602739725</v>
       </c>
       <c r="R13">
@@ -4722,6 +4783,9 @@
         <v>0</v>
       </c>
       <c r="U13">
+        <v>2</v>
+      </c>
+      <c r="V13">
         <v>2</v>
       </c>
       <c r="W13">
@@ -4770,6 +4834,9 @@
       <c r="U14">
         <v>2</v>
       </c>
+      <c r="V14">
+        <v>3</v>
+      </c>
       <c r="W14">
         <v>9.11E-2</v>
       </c>
@@ -4834,6 +4901,9 @@
       <c r="U16">
         <v>3</v>
       </c>
+      <c r="V16">
+        <v>4</v>
+      </c>
       <c r="W16">
         <v>1.8020000000000001E-2</v>
       </c>
@@ -4883,6 +4953,9 @@
       <c r="U17">
         <v>3</v>
       </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
       <c r="W17">
         <v>1.3089999999999999E-2</v>
       </c>
@@ -4937,6 +5010,9 @@
       </c>
       <c r="U19">
         <v>4</v>
+      </c>
+      <c r="V19">
+        <v>6</v>
       </c>
       <c r="W19">
         <v>3.49E-2</v>
@@ -5004,6 +5080,9 @@
       <c r="U21">
         <v>4</v>
       </c>
+      <c r="V21">
+        <v>7</v>
+      </c>
       <c r="W21">
         <v>3.0300000000000001E-2</v>
       </c>
@@ -5047,6 +5126,9 @@
       <c r="U22">
         <v>4</v>
       </c>
+      <c r="V22">
+        <v>8</v>
+      </c>
       <c r="W22">
         <v>1.4E-2</v>
       </c>
@@ -5102,6 +5184,9 @@
       <c r="U24">
         <v>4</v>
       </c>
+      <c r="V24">
+        <v>9</v>
+      </c>
       <c r="W24">
         <v>1.9400000000000001E-2</v>
       </c>
@@ -5145,6 +5230,9 @@
       <c r="U25">
         <v>4</v>
       </c>
+      <c r="V25">
+        <v>10</v>
+      </c>
       <c r="W25" s="4">
         <v>1.1610000000000001E-2</v>
       </c>
@@ -5206,6 +5294,9 @@
       <c r="U26">
         <v>4</v>
       </c>
+      <c r="V26">
+        <v>11</v>
+      </c>
       <c r="W26">
         <v>1.6400000000000001E-2</v>
       </c>
@@ -5249,6 +5340,9 @@
       <c r="U27">
         <v>4</v>
       </c>
+      <c r="V27">
+        <v>12</v>
+      </c>
       <c r="W27">
         <v>1.1599999999999999E-2</v>
       </c>
@@ -5310,6 +5404,9 @@
       <c r="T28">
         <v>0</v>
       </c>
+      <c r="V28">
+        <v>13</v>
+      </c>
       <c r="W28">
         <v>1.43E-2</v>
       </c>
@@ -5445,6 +5542,9 @@
       <c r="T32">
         <v>1</v>
       </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
       <c r="V32" s="3">
         <v>0.61909848000000001</v>
       </c>
@@ -5493,6 +5593,9 @@
       <c r="T33">
         <v>1</v>
       </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
       <c r="V33" s="3">
         <v>0.23714600999999999</v>
       </c>
@@ -5532,7 +5635,7 @@
         <v>256</v>
       </c>
       <c r="P35">
-        <f t="shared" ref="P34:P36" si="2">$C$6/(H35-I35)</f>
+        <f t="shared" ref="P35:P36" si="2">$C$6/(H35-I35)</f>
         <v>86.705202312138724</v>
       </c>
       <c r="Q35">
@@ -5545,6 +5648,9 @@
         <v>0</v>
       </c>
       <c r="T35">
+        <v>2</v>
+      </c>
+      <c r="U35">
         <v>2</v>
       </c>
       <c r="V35" s="3">
@@ -5595,6 +5701,9 @@
       <c r="T36">
         <v>2</v>
       </c>
+      <c r="U36">
+        <v>3</v>
+      </c>
       <c r="V36" s="3">
         <v>0.21716887000000001</v>
       </c>
@@ -5648,6 +5757,9 @@
       <c r="T38">
         <v>3</v>
       </c>
+      <c r="U38">
+        <v>4</v>
+      </c>
       <c r="V38" s="3">
         <v>1.406466E-2</v>
       </c>
@@ -5686,6 +5798,9 @@
       <c r="T39">
         <v>3</v>
       </c>
+      <c r="U39">
+        <v>5</v>
+      </c>
       <c r="V39" s="3">
         <v>1.943139E-2</v>
       </c>
@@ -5739,6 +5854,9 @@
       <c r="S41">
         <v>2</v>
       </c>
+      <c r="U41">
+        <v>6</v>
+      </c>
       <c r="V41" s="3">
         <v>5.2009400000000003E-3</v>
       </c>
@@ -5771,6 +5889,9 @@
       <c r="S42">
         <v>3</v>
       </c>
+      <c r="U42">
+        <v>7</v>
+      </c>
       <c r="V42" s="3">
         <v>5.2009500000000002E-3</v>
       </c>
@@ -5806,6 +5927,9 @@
       <c r="S43">
         <v>4</v>
       </c>
+      <c r="U43">
+        <v>8</v>
+      </c>
       <c r="V43" s="3">
         <v>5.1623780000000001E-2</v>
       </c>
@@ -5856,6 +5980,9 @@
       <c r="S44">
         <v>5</v>
       </c>
+      <c r="U44">
+        <v>9</v>
+      </c>
       <c r="V44" s="3">
         <v>5.0428000000000001E-3</v>
       </c>
@@ -5864,6 +5991,12 @@
       </c>
     </row>
     <row r="45" spans="3:24">
+      <c r="H45">
+        <v>3550</v>
+      </c>
+      <c r="I45">
+        <v>130</v>
+      </c>
       <c r="L45">
         <v>42.9</v>
       </c>
@@ -5878,6 +6011,9 @@
       </c>
       <c r="S45">
         <v>6</v>
+      </c>
+      <c r="U45">
+        <v>10</v>
       </c>
       <c r="V45" s="3">
         <v>6.8193200000000002E-3</v>
@@ -5913,6 +6049,9 @@
       </c>
       <c r="S46">
         <v>7</v>
+      </c>
+      <c r="U46">
+        <v>11</v>
       </c>
       <c r="V46" s="3">
         <v>1.379608E-2</v>
@@ -5929,7 +6068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6260,7 +6399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A4:U31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6750,7 +6889,7 @@
         <v>256</v>
       </c>
       <c r="Q26">
-        <f>250000/(I26-J26)</f>
+        <f t="shared" ref="Q26:Q31" si="0">250000/(I26-J26)</f>
         <v>84.459459459459453</v>
       </c>
       <c r="R26">
@@ -6792,7 +6931,7 @@
         <v>256</v>
       </c>
       <c r="Q27">
-        <f>250000/(I27-J27)</f>
+        <f t="shared" si="0"/>
         <v>77.639751552795033</v>
       </c>
       <c r="R27">
@@ -6837,7 +6976,7 @@
         <v>256</v>
       </c>
       <c r="Q28">
-        <f>250000/(I28-J28)</f>
+        <f t="shared" si="0"/>
         <v>76.452599388379198</v>
       </c>
       <c r="R28">
@@ -6879,7 +7018,7 @@
         <v>256</v>
       </c>
       <c r="Q29">
-        <f>250000/(I29-J29)</f>
+        <f t="shared" si="0"/>
         <v>81.433224755700323</v>
       </c>
       <c r="R29">
@@ -6933,7 +7072,7 @@
         <v>256</v>
       </c>
       <c r="Q30">
-        <f>250000/(I30-J30)</f>
+        <f t="shared" si="0"/>
         <v>81.433224755700323</v>
       </c>
       <c r="R30">
@@ -6972,7 +7111,7 @@
         <v>256</v>
       </c>
       <c r="Q31">
-        <f>250000/(I31-J31)</f>
+        <f t="shared" si="0"/>
         <v>81.433224755700323</v>
       </c>
       <c r="R31">
@@ -6988,7 +7127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="D4:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
ploty do diplomky + kompletni vypocet shiftu
</commit_message>
<xml_diff>
--- a/EMM_minim/algoritmus minimalizace/EMM_min_pomocne_data.xlsx
+++ b/EMM_minim/algoritmus minimalizace/EMM_min_pomocne_data.xlsx
@@ -857,7 +857,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1198,7 +1197,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4811,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B331" sqref="B331"/>
+    <sheetView tabSelected="1" topLeftCell="H310" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H313" sqref="H313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10600,14 +10598,14 @@
         <v>50</v>
       </c>
       <c r="O195" s="11">
-        <f t="shared" ref="O194:O207" si="13">(K195-L195)/(K195+L195)</f>
+        <f t="shared" ref="O195:O207" si="13">(K195-L195)/(K195+L195)</f>
         <v>0.13800000000000001</v>
       </c>
       <c r="P195" s="16">
         <v>256</v>
       </c>
       <c r="Q195" s="8">
-        <f t="shared" ref="Q194:Q205" si="14" xml:space="preserve"> $C$187/(I195-J195)</f>
+        <f t="shared" ref="Q195:Q205" si="14" xml:space="preserve"> $C$187/(I195-J195)</f>
         <v>86.206896551724142</v>
       </c>
       <c r="R195" s="16">
@@ -11260,7 +11258,7 @@
         <v>256</v>
       </c>
       <c r="P214" s="11">
-        <f t="shared" ref="P213:P215" si="15">$C$187/(H214-I214)</f>
+        <f t="shared" ref="P214:P215" si="15">$C$187/(H214-I214)</f>
         <v>79.617834394904463</v>
       </c>
       <c r="Q214" s="16">
@@ -11771,7 +11769,7 @@
         <v>256</v>
       </c>
       <c r="P236" s="11">
-        <f t="shared" ref="P235:P240" si="16">$C$187/(H236-I236)</f>
+        <f t="shared" ref="P236:P240" si="16">$C$187/(H236-I236)</f>
         <v>113.63636363636364</v>
       </c>
       <c r="Q236">
@@ -12622,7 +12620,7 @@
         <v>50</v>
       </c>
       <c r="O276" s="11">
-        <f t="shared" ref="O275:O287" si="17">(K276-L276)/(K276+L276)</f>
+        <f t="shared" ref="O276:O287" si="17">(K276-L276)/(K276+L276)</f>
         <v>0.13800000000000001</v>
       </c>
       <c r="P276" s="16">

</xml_diff>